<commit_message>
Implemented file writer to write processed transactions into excel and added a line in driver to run this method
</commit_message>
<xml_diff>
--- a/TestFiles/TransactionReport.xlsx
+++ b/TestFiles/TransactionReport.xlsx
@@ -12,9 +12,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
-  <si>
-    <t>Transaction</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Description</t>
   </si>
   <si>
     <t>Credit</t>
@@ -23,22 +26,55 @@
     <t>Debit</t>
   </si>
   <si>
-    <t>Effective Java</t>
-  </si>
-  <si>
-    <t>Joshua Bloch</t>
-  </si>
-  <si>
-    <t>Clean Code</t>
-  </si>
-  <si>
-    <t>Robert martin</t>
-  </si>
-  <si>
-    <t>Thinking in Java</t>
-  </si>
-  <si>
-    <t>Bruce Eckel</t>
+    <t>Buyer</t>
+  </si>
+  <si>
+    <t>Tag</t>
+  </si>
+  <si>
+    <t>10/22/2019</t>
+  </si>
+  <si>
+    <t>LOBLAWS #1066</t>
+  </si>
+  <si>
+    <t>JP</t>
+  </si>
+  <si>
+    <t>Prescriptions</t>
+  </si>
+  <si>
+    <t>10/23/2019</t>
+  </si>
+  <si>
+    <t>SOBEYS 849       QPS</t>
+  </si>
+  <si>
+    <t>CW</t>
+  </si>
+  <si>
+    <t>sobeys</t>
+  </si>
+  <si>
+    <t>THE ORIGINAL MOM'S RESTAU</t>
+  </si>
+  <si>
+    <t>OP</t>
+  </si>
+  <si>
+    <t>food</t>
+  </si>
+  <si>
+    <t>10/24/2019</t>
+  </si>
+  <si>
+    <t>METRO #704</t>
+  </si>
+  <si>
+    <t>GI</t>
+  </si>
+  <si>
+    <t>Gas</t>
   </si>
 </sst>
 </file>
@@ -83,7 +119,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -99,38 +135,94 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C2" t="n">
-        <v>36.0</v>
+        <v>62.78</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="E2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="C3" t="n">
-        <v>42.0</v>
+        <v>42.69</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="E3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C4" t="n">
-        <v>35.0</v>
+        <v>78.11</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="E4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" t="n">
+        <v>46.77</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="E5" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>